<commit_message>
inputs validation updated with case
</commit_message>
<xml_diff>
--- a/data/Inputs_Validation.xlsx
+++ b/data/Inputs_Validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B94AC570-58BD-4071-B322-0F83A50A0FE5}"/>
+  <xr:revisionPtr revIDLastSave="418" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3475D75-BE64-4155-991D-CA0354D0AED6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" activeTab="9" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -70,14 +70,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>B1</t>
   </si>
   <si>
-    <t>B2</t>
-  </si>
-  <si>
     <t>distance</t>
   </si>
   <si>
@@ -147,18 +144,6 @@
     <t>cost_charter_day</t>
   </si>
   <si>
-    <t>cost_purchase</t>
-  </si>
-  <si>
-    <t>cost_operation</t>
-  </si>
-  <si>
-    <t>cost_technicians</t>
-  </si>
-  <si>
-    <t>cost_downtime</t>
-  </si>
-  <si>
     <t>penalty_cost_late</t>
   </si>
   <si>
@@ -186,13 +171,28 @@
     <t>max_capacity_for_docking</t>
   </si>
   <si>
-    <t>additional_time</t>
-  </si>
-  <si>
-    <t>tech_standby_cost</t>
-  </si>
-  <si>
     <t>initial_inventory</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>PRE</t>
   </si>
 </sst>
 </file>
@@ -570,80 +570,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF71955-FB00-4A13-9841-9B985EEEFB62}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>365</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>365</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>500</v>
+        <v>1000000</v>
       </c>
       <c r="F2">
-        <v>200000</v>
-      </c>
-      <c r="G2">
-        <v>1000000</v>
-      </c>
-      <c r="H2">
-        <v>80</v>
-      </c>
-      <c r="I2">
-        <v>20</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -654,39 +634,33 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EB2CC8-B9D8-4FE5-960B-9B0984034D8D}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
         <v>B1</v>
       </c>
       <c r="C1" t="str">
-        <v>B2</v>
-      </c>
-      <c r="D1" t="str">
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -696,27 +670,45 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EDE46-A218-4D87-9847-C01D7AFA5102}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:E1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
         <v>M1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="str">
+        <v>M2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>M3</v>
+      </c>
+      <c r="E1" t="str">
+        <v>M4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -726,39 +718,33 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053CB446-56D8-4850-8B54-9A701C7360FF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
         <v>B1</v>
       </c>
       <c r="C1" t="str">
-        <v>B2</v>
-      </c>
-      <c r="D1" t="str">
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>300</v>
-      </c>
-      <c r="D2">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -771,36 +757,33 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:D1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
         <v>B1</v>
       </c>
       <c r="C1" t="str">
-        <v>B2</v>
-      </c>
-      <c r="D1" t="str">
         <v>V4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
         <v>S1</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -810,58 +793,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E241-D090-4C23-9A88-3F3C92E70F61}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>550000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>80</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>450000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -871,78 +833,69 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D2">
         <v>20</v>
       </c>
       <c r="E2">
-        <v>166.67</v>
+        <v>1750</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <f>15/60</f>
@@ -954,56 +907,122 @@
       <c r="I2">
         <v>12</v>
       </c>
-      <c r="J2">
-        <v>10000</v>
-      </c>
-      <c r="K2">
-        <v>166.67</v>
-      </c>
-      <c r="L2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>5000</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>0.25</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>12500</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>0.25</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2.5</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>25000</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>800</v>
-      </c>
-      <c r="F3">
-        <v>40</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>168</v>
-      </c>
-      <c r="J3">
-        <v>20000</v>
-      </c>
-      <c r="K3">
-        <v>50</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>0.15</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>336</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1015,22 +1034,22 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(vessels!A2:A100, vessels!B2:B100 = 1)</f>
+        <f t="array" ref="A2">_xlfn._xlws.FILTER(vessels!A2:A98, vessels!B2:B98 = 1)</f>
         <v>V4</v>
       </c>
     </row>
@@ -1041,89 +1060,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABC1D42-2EA6-4A74-ACE3-149C8A508F63}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A4">_xlfn.LET(
+        <f t="array" ref="A2:A3">_xlfn.LET(
     _xlpm.baseList, _xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100 &lt;&gt; ""),
-    _xlpm.vesselList, _xlfn._xlws.FILTER(vessels!A2:A100, vessels!B2:B100 = 1),
+    _xlpm.vesselList, _xlfn._xlws.FILTER(vessels!A2:A98, vessels!B2:B98 = 1),
     _xlfn.VSTACK(_xlpm.baseList, _xlpm.vesselList)
 )</f>
         <v>B1</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <v>B2</v>
+        <v>V4</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <v>V4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
         <v>0</v>
       </c>
     </row>
@@ -1134,49 +1136,49 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF4AD3B-D68B-43E0-80DF-E258B870C86F}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1185,13 +1187,82 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="F2">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>7.5</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="F4">
+        <v>18500</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>18500</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1204,31 +1275,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1238,33 +1309,111 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F60F74-5991-4DF7-ADB4-D8FEE6BDA60A}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:F1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A98, vessels!A2:A98&lt;&gt;""))</f>
         <v>V1</v>
       </c>
       <c r="C1" t="str">
+        <v>V2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>V3</v>
+      </c>
+      <c r="E1" t="str">
         <v>V4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="str">
+        <v>V5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;"")</f>
+        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;"")</f>
         <v>M1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <v>M2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>M3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <v>M4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1274,44 +1423,51 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3E7950-5805-40E5-8CB7-09BB0C8D59D5}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A100, vessels!A2:A100&lt;&gt;""))</f>
+        <f t="array" ref="B1:F1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A98, vessels!A2:A98&lt;&gt;""))</f>
         <v>V1</v>
       </c>
       <c r="C1" t="str">
+        <v>V2</v>
+      </c>
+      <c r="D1" t="str">
+        <v>V3</v>
+      </c>
+      <c r="E1" t="str">
         <v>V4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="str">
+        <v>V5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A3">_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;"")</f>
+        <f t="array" ref="A2">_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;"")</f>
         <v>B1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <v>B2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validation with mothervessels performing tasks and good results?
</commit_message>
<xml_diff>
--- a/data/Inputs_Validation.xlsx
+++ b/data/Inputs_Validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="437" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0134AF7D-5975-4ABF-8F82-9E3DD5DB08B7}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0481EC8-6A01-454A-85AF-1F4840E14893}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" firstSheet="4" activeTab="4" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" firstSheet="1" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABC1D42-2EA6-4A74-ACE3-149C8A508F63}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1495,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1515,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>

</xml_diff>

<commit_message>
Ready for remote runs
</commit_message>
<xml_diff>
--- a/data/Inputs_Validation.xlsx
+++ b/data/Inputs_Validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3dd903d477a9e4d/02_ME/ME54015/OWF_Vessel-Fleet-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="441" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0481EC8-6A01-454A-85AF-1F4840E14893}"/>
+  <xr:revisionPtr revIDLastSave="490" documentId="13_ncr:1_{4E655DA3-6644-44D5-B8A3-390376DF86AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC03D96F-1328-4204-A3B9-4EB7B3C544A1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" firstSheet="1" activeTab="2" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="853" activeTab="1" xr2:uid="{5CDB4E5C-34BF-4466-8F20-CB91BE55E2BE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -48,30 +48,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="40">
   <si>
     <t>B1</t>
   </si>
@@ -635,33 +613,31 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:F1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A98, vessels!A2:A98&lt;&gt;""))</f>
-        <v>V1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>V2</v>
-      </c>
-      <c r="D1" t="str">
-        <v>V3</v>
-      </c>
-      <c r="E1" t="str">
-        <v>V4</v>
-      </c>
-      <c r="F1" t="str">
-        <v>V5</v>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100&lt;&gt;"")</f>
-        <v>B1</v>
+      <c r="A2" t="s">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -689,24 +665,22 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
-        <v>B1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>V4</v>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -725,30 +699,28 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:E1">TRANSPOSE(_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;""))</f>
-        <v>M1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>M2</v>
-      </c>
-      <c r="D1" t="str">
-        <v>M3</v>
-      </c>
-      <c r="E1" t="str">
-        <v>M4</v>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -773,24 +745,22 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
-        <v>B1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>V4</v>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -806,35 +776,30 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899CD8D2-6DC6-477C-BD52-3078DFB872A3}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:C1">TRANSPOSE(_xlfn._xlws.FILTER(locations!A2:A100, locations!A2:A100&lt;&gt;""))</f>
-        <v>B1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>V4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(spare_parts!A2:A100, spare_parts!A2:A100&lt;&gt;"")</f>
-        <v>S1</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
         <v>0</v>
       </c>
     </row>
@@ -847,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E241-D090-4C23-9A88-3F3C92E70F61}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5129D5-4392-4795-B324-B7E69B03092B}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,7 +1051,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,9 +1065,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.FILTER(vessels!A2:A98, vessels!B2:B98 = 1)</f>
-        <v>V4</v>
+      <c r="A2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1115,7 +1079,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,13 +1103,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A3">_xlfn.LET(
-    _xlpm.baseList, _xlfn._xlws.FILTER(bases!A2:A100, bases!A2:A100 &lt;&gt; ""),
-    _xlpm.vesselList, _xlfn._xlws.FILTER(vessels!A2:A98, vessels!B2:B98 = 1),
-    _xlfn.VSTACK(_xlpm.baseList, _xlpm.vesselList)
-)</f>
-        <v>B1</v>
+      <c r="A2" t="s">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -1158,8 +1117,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>V4</v>
+      <c r="A3" t="s">
+        <v>31</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1181,7 +1140,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="A2:XFD2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1203,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,7 +1339,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1417,33 +1376,31 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:F1">TRANSPOSE(_xlfn._xlws.FILTER(vessels!A2:A98, vessels!A2:A98&lt;&gt;""))</f>
-        <v>V1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>V2</v>
-      </c>
-      <c r="D1" t="str">
-        <v>V3</v>
-      </c>
-      <c r="E1" t="str">
-        <v>V4</v>
-      </c>
-      <c r="F1" t="str">
-        <v>V5</v>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A5">_xlfn._xlws.FILTER(tasks!A2:A100, tasks!A2:A100&lt;&gt;"")</f>
-        <v>M1</v>
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1462,8 +1419,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <v>M2</v>
+      <c r="A3" t="s">
+        <v>36</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1482,8 +1439,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <v>M3</v>
+      <c r="A4" t="s">
+        <v>37</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1502,8 +1459,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <v>M4</v>
+      <c r="A5" t="s">
+        <v>38</v>
       </c>
       <c r="B5">
         <v>1</v>

</xml_diff>